<commit_message>
Coreciones Diseño Exportacion XLSX
</commit_message>
<xml_diff>
--- a/util/plantillas/template-report.xlsx
+++ b/util/plantillas/template-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\GDBackEnd\util\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E50118B-91C1-4AEF-8E12-00B6C3E58603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85671267-8E9C-4FEC-83AE-C41BDE80A4D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts" sheetId="2" r:id="rId1"/>
@@ -46,18 +46,12 @@
     <t>Detail</t>
   </si>
   <si>
-    <t>Initial_balance</t>
-  </si>
-  <si>
     <t>Sign</t>
   </si>
   <si>
     <t>Income</t>
   </si>
   <si>
-    <t>Expsense</t>
-  </si>
-  <si>
     <t>Balance</t>
   </si>
   <si>
@@ -122,6 +116,12 @@
   </si>
   <si>
     <t>Movements</t>
+  </si>
+  <si>
+    <t>Initial Balance</t>
+  </si>
+  <si>
+    <t>Expense</t>
   </si>
 </sst>
 </file>
@@ -248,13 +248,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,55 +540,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A586D2-BEB9-494D-B82E-A04D8295D91D}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
+    <col min="5" max="7" width="25.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -598,22 +596,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -632,104 +630,101 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="25.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -747,57 +742,56 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:E4"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2"/>
-    <col min="4" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" style="2" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -815,43 +809,43 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:C4"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="34.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23" style="2" customWidth="1"/>
+    <col min="1" max="2" width="35.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -869,37 +863,37 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
     <col min="3" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -916,70 +910,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB5F2E8-308D-4342-8F93-1619AA3FF0DE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="22.85546875" style="2" customWidth="1"/>
+    <col min="1" max="3" width="25.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>